<commit_message>
Now using a 50Hz timer, instead of BPMs to change the lines and play notes. The effects are applied on the 50Hz timer, even when notes are not played.
</commit_message>
<xml_diff>
--- a/bpm-to-timer-count.xlsx
+++ b/bpm-to-timer-count.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\foenix\c256-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{4FF7B1DA-B787-46F6-B80F-EB5311328D82}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE3B5D7-4C65-48AB-A60C-19BCB67DB42B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16665" yWindow="4995" windowWidth="43200" windowHeight="17175" xr2:uid="{9DD0EEA4-90D0-417E-9B15-B3E3E0911043}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{9DD0EEA4-90D0-417E-9B15-B3E3E0911043}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>bpm</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>369E6</t>
+  </si>
+  <si>
+    <t>Interrupt every</t>
+  </si>
+  <si>
+    <t>RAD Timer (Hz)</t>
+  </si>
+  <si>
+    <t>CPU Clock (Hz)</t>
   </si>
 </sst>
 </file>
@@ -453,19 +462,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD58F71A-EA66-40FB-8BC7-6B4B15E74342}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D44"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,8 +485,18 @@
       <c r="C1">
         <v>14318000</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1">
+        <v>50</v>
+      </c>
+      <c r="H1">
+        <f>1/G1</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>60</v>
       </c>
@@ -492,25 +512,31 @@
         <f>DEC2HEX(C2)</f>
         <v>DA79B</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2">
+        <v>14318000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>120</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B43" si="0">A3*16/60</f>
+        <f t="shared" ref="B3:B22" si="0">A3*16/60</f>
         <v>32</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C44" si="1">1/B3 * $C$1</f>
+        <f t="shared" ref="C3:C22" si="1">1/B3 * $C$1</f>
         <v>447437.5</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D44" si="2">DEC2HEX(C3)</f>
+        <f t="shared" ref="D3:D22" si="2">DEC2HEX(C3)</f>
         <v>6D3CD</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>200</v>
       </c>
@@ -526,8 +552,15 @@
         <f t="shared" si="2"/>
         <v>418AE</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <f>H1 * G2</f>
+        <v>286360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>201</v>
       </c>
@@ -544,7 +577,7 @@
         <v>41376</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>202</v>
       </c>
@@ -561,7 +594,7 @@
         <v>40E4C</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>203</v>
       </c>
@@ -578,7 +611,7 @@
         <v>4092F</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>204</v>
       </c>
@@ -595,7 +628,7 @@
         <v>4041E</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>205</v>
       </c>
@@ -612,7 +645,7 @@
         <v>3FF1A</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>206</v>
       </c>
@@ -629,7 +662,7 @@
         <v>3FA23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>207</v>
       </c>
@@ -646,7 +679,7 @@
         <v>3F538</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>208</v>
       </c>
@@ -663,7 +696,7 @@
         <v>3F059</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>209</v>
       </c>
@@ -680,7 +713,7 @@
         <v>3EB85</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>210</v>
       </c>
@@ -697,7 +730,7 @@
         <v>3E6BE</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>211</v>
       </c>
@@ -714,7 +747,7 @@
         <v>3E202</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>212</v>
       </c>
@@ -731,7 +764,7 @@
         <v>3DD52</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>213</v>
       </c>
@@ -748,7 +781,7 @@
         <v>3D8AD</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>214</v>
       </c>
@@ -765,7 +798,7 @@
         <v>3D413</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>215</v>
       </c>
@@ -782,7 +815,7 @@
         <v>3CF84</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>216</v>
       </c>
@@ -799,7 +832,7 @@
         <v>3CB00</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>217</v>
       </c>
@@ -816,7 +849,7 @@
         <v>3C686</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>218</v>
       </c>
@@ -833,7 +866,7 @@
         <v>3C217</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>219</v>
       </c>
@@ -847,7 +880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>220</v>
       </c>
@@ -861,7 +894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>221</v>
       </c>
@@ -875,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>222</v>
       </c>
@@ -889,7 +922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>223</v>
       </c>
@@ -903,7 +936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>224</v>
       </c>
@@ -917,7 +950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>225</v>
       </c>
@@ -931,7 +964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>226</v>
       </c>
@@ -945,7 +978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>227</v>
       </c>
@@ -959,7 +992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>228</v>
       </c>
@@ -973,7 +1006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>229</v>
       </c>
@@ -987,7 +1020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>230</v>
       </c>
@@ -1001,7 +1034,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>231</v>
       </c>
@@ -1015,7 +1048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>232</v>
       </c>
@@ -1029,7 +1062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>233</v>
       </c>
@@ -1043,7 +1076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>234</v>
       </c>
@@ -1057,7 +1090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>235</v>
       </c>
@@ -1071,7 +1104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>236</v>
       </c>
@@ -1085,7 +1118,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>237</v>
       </c>
@@ -1099,7 +1132,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>238</v>
       </c>
@@ -1113,7 +1146,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>239</v>
       </c>
@@ -1127,7 +1160,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>240</v>
       </c>

</xml_diff>

<commit_message>
Modified for Vicky II - mostly display width changes.
</commit_message>
<xml_diff>
--- a/bpm-to-timer-count.xlsx
+++ b/bpm-to-timer-count.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\foenix\c256-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE3B5D7-4C65-48AB-A60C-19BCB67DB42B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E11D51C-DB57-4E5A-8FB5-50C761E56EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{9DD0EEA4-90D0-417E-9B15-B3E3E0911043}"/>
+    <workbookView xWindow="5040" yWindow="3900" windowWidth="23100" windowHeight="15225" xr2:uid="{9DD0EEA4-90D0-417E-9B15-B3E3E0911043}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>bpm</t>
   </si>
@@ -111,6 +112,12 @@
   </si>
   <si>
     <t>CPU Clock (Hz)</t>
+  </si>
+  <si>
+    <t>8kHz</t>
+  </si>
+  <si>
+    <t>48kHz</t>
   </si>
 </sst>
 </file>
@@ -462,20 +469,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD58F71A-EA66-40FB-8BC7-6B4B15E74342}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +503,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>60</v>
       </c>
@@ -518,8 +525,15 @@
       <c r="G2">
         <v>14318000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <f>G2/8000</f>
+        <v>1789.75</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>120</v>
       </c>
@@ -535,8 +549,15 @@
         <f t="shared" ref="D3:D22" si="2">DEC2HEX(C3)</f>
         <v>6D3CD</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <f>G2/48000</f>
+        <v>298.29166666666669</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>200</v>
       </c>
@@ -560,7 +581,7 @@
         <v>286360</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>201</v>
       </c>
@@ -577,7 +598,7 @@
         <v>41376</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>202</v>
       </c>
@@ -594,7 +615,7 @@
         <v>40E4C</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>203</v>
       </c>
@@ -611,7 +632,7 @@
         <v>4092F</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>204</v>
       </c>
@@ -628,7 +649,7 @@
         <v>4041E</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>205</v>
       </c>
@@ -645,7 +666,7 @@
         <v>3FF1A</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>206</v>
       </c>
@@ -662,7 +683,7 @@
         <v>3FA23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>207</v>
       </c>
@@ -679,7 +700,7 @@
         <v>3F538</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>208</v>
       </c>
@@ -696,7 +717,7 @@
         <v>3F059</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>209</v>
       </c>
@@ -713,7 +734,7 @@
         <v>3EB85</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>210</v>
       </c>
@@ -730,7 +751,7 @@
         <v>3E6BE</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>211</v>
       </c>
@@ -747,7 +768,7 @@
         <v>3E202</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>212</v>
       </c>
@@ -764,7 +785,7 @@
         <v>3DD52</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>213</v>
       </c>
@@ -781,7 +802,7 @@
         <v>3D8AD</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>214</v>
       </c>
@@ -798,7 +819,7 @@
         <v>3D413</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>215</v>
       </c>
@@ -815,7 +836,7 @@
         <v>3CF84</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>216</v>
       </c>
@@ -832,7 +853,7 @@
         <v>3CB00</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>217</v>
       </c>
@@ -849,7 +870,7 @@
         <v>3C686</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>218</v>
       </c>
@@ -866,7 +887,7 @@
         <v>3C217</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>219</v>
       </c>
@@ -880,7 +901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>220</v>
       </c>
@@ -894,7 +915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>221</v>
       </c>
@@ -908,7 +929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>222</v>
       </c>
@@ -922,7 +943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>223</v>
       </c>
@@ -936,7 +957,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>224</v>
       </c>
@@ -950,7 +971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>225</v>
       </c>
@@ -964,7 +985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>226</v>
       </c>
@@ -978,7 +999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>227</v>
       </c>
@@ -992,7 +1013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>228</v>
       </c>
@@ -1006,7 +1027,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>229</v>
       </c>
@@ -1020,7 +1041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>230</v>
       </c>
@@ -1034,7 +1055,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>231</v>
       </c>
@@ -1048,7 +1069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>232</v>
       </c>
@@ -1062,7 +1083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>233</v>
       </c>
@@ -1076,7 +1097,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>234</v>
       </c>
@@ -1090,7 +1111,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>235</v>
       </c>
@@ -1104,7 +1125,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>236</v>
       </c>
@@ -1118,7 +1139,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>237</v>
       </c>
@@ -1132,7 +1153,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>238</v>
       </c>
@@ -1146,7 +1167,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>239</v>
       </c>
@@ -1160,7 +1181,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>240</v>
       </c>

</xml_diff>

<commit_message>
Release 0.4.0 ------------- Added FAT32 support. Added Vicky II display format.
</commit_message>
<xml_diff>
--- a/bpm-to-timer-count.xlsx
+++ b/bpm-to-timer-count.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\foenix\c256-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E11D51C-DB57-4E5A-8FB5-50C761E56EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB5B4B5-125A-40A1-9C83-BD07C6557DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="3900" windowWidth="23100" windowHeight="15225" xr2:uid="{9DD0EEA4-90D0-417E-9B15-B3E3E0911043}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="18816" xr2:uid="{9DD0EEA4-90D0-417E-9B15-B3E3E0911043}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>bpm</t>
   </si>
@@ -118,14 +119,52 @@
   </si>
   <si>
     <t>48kHz</t>
+  </si>
+  <si>
+    <t>Timer Value</t>
+  </si>
+  <si>
+    <t>µs per qtr</t>
+  </si>
+  <si>
+    <t>qtr per sec</t>
+  </si>
+  <si>
+    <t>BPM</t>
+  </si>
+  <si>
+    <t>ticks per quarter</t>
+  </si>
+  <si>
+    <t>us per quarter</t>
+  </si>
+  <si>
+    <t>us per tick</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t>max wait</t>
+  </si>
+  <si>
+    <t>44.1KHz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -153,8 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,27 +514,31 @@
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
         <v>14318000</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G1">
@@ -503,7 +549,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>60</v>
       </c>
@@ -519,7 +565,7 @@
         <f>DEC2HEX(C2)</f>
         <v>DA79B</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G2">
@@ -533,7 +579,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>120</v>
       </c>
@@ -542,11 +588,11 @@
         <v>32</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C22" si="1">1/B3 * $C$1</f>
+        <f>1/B3 * $C$1</f>
         <v>447437.5</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D22" si="2">DEC2HEX(C3)</f>
+        <f t="shared" ref="D3:D22" si="1">DEC2HEX(C3)</f>
         <v>6D3CD</v>
       </c>
       <c r="J3">
@@ -557,7 +603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>200</v>
       </c>
@@ -566,11 +612,11 @@
         <v>53.333333333333336</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C4:C22" si="2">1/B4 * $C$1</f>
         <v>268462.5</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>418AE</v>
       </c>
       <c r="F4" t="s">
@@ -580,8 +626,15 @@
         <f>H1 * G2</f>
         <v>286360</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f>G2/44100</f>
+        <v>324.67120181405897</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>201</v>
       </c>
@@ -590,15 +643,15 @@
         <v>53.6</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>267126.86567164178</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>41376</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>202</v>
       </c>
@@ -607,15 +660,15 @@
         <v>53.866666666666667</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>265804.45544554456</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40E4C</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>203</v>
       </c>
@@ -624,15 +677,24 @@
         <v>54.133333333333333</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>264495.07389162562</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4092F</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>204</v>
       </c>
@@ -641,15 +703,30 @@
         <v>54.4</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>263198.5294117647</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4041E</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H8">
+        <f>1/G8</f>
+        <v>2.5</v>
+      </c>
+      <c r="I8">
+        <f>H8*60</f>
+        <v>150</v>
+      </c>
+      <c r="K8" s="3">
+        <f>60/G8</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>205</v>
       </c>
@@ -658,15 +735,30 @@
         <v>54.666666666666664</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>261914.6341463415</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3FF1A</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G9" s="2">
+        <v>0.28571400000000002</v>
+      </c>
+      <c r="H9">
+        <f>1/G9</f>
+        <v>3.5000035000034999</v>
+      </c>
+      <c r="I9">
+        <f>H9*60</f>
+        <v>210.00021000020999</v>
+      </c>
+      <c r="K9" s="3">
+        <f>60/G9</f>
+        <v>210.00021000020999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>206</v>
       </c>
@@ -675,15 +767,15 @@
         <v>54.93333333333333</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>260643.20388349518</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3FA23</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>207</v>
       </c>
@@ -692,15 +784,15 @@
         <v>55.2</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>259384.0579710145</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3F538</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>208</v>
       </c>
@@ -709,15 +801,15 @@
         <v>55.466666666666669</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>258137.01923076922</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3F059</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>209</v>
       </c>
@@ -726,15 +818,15 @@
         <v>55.733333333333334</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>256901.91387559808</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3EB85</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>210</v>
       </c>
@@ -743,15 +835,15 @@
         <v>56</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>255678.57142857142</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3E6BE</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>211</v>
       </c>
@@ -760,15 +852,21 @@
         <v>56.266666666666666</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>254466.82464454975</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3E202</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>240</v>
+      </c>
+      <c r="H15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>212</v>
       </c>
@@ -777,15 +875,21 @@
         <v>56.533333333333331</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>253266.50943396226</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3DD52</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>285714</v>
+      </c>
+      <c r="H16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>213</v>
       </c>
@@ -794,15 +898,22 @@
         <v>56.8</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>252077.46478873241</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3D8AD</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f>G16/G15</f>
+        <v>1190.4749999999999</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>214</v>
       </c>
@@ -811,15 +922,22 @@
         <v>57.06666666666667</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250899.53271028036</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3D413</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>44100</v>
+      </c>
+      <c r="H18" s="3">
+        <f>1/G18 * 1000000</f>
+        <v>22.675736961451246</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>215</v>
       </c>
@@ -828,7 +946,7 @@
         <v>57.333333333333336</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>249732.55813953487</v>
       </c>
       <c r="D19" t="str">
@@ -836,7 +954,7 @@
         <v>3CF84</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>216</v>
       </c>
@@ -845,15 +963,22 @@
         <v>57.6</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>248576.38888888891</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3CB00</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="3">
+        <f>G17 * G18 /1000000</f>
+        <v>52.49994749999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>217</v>
       </c>
@@ -862,15 +987,15 @@
         <v>57.866666666666667</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>247430.87557603689</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3C686</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>218</v>
       </c>
@@ -879,15 +1004,15 @@
         <v>58.133333333333333</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>246295.87155963303</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3C217</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>219</v>
       </c>
@@ -900,8 +1025,18 @@
       <c r="D23" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>65535</v>
+      </c>
+      <c r="H23">
+        <f>H18*G23 / 1000000</f>
+        <v>1.4860544217687075</v>
+      </c>
+      <c r="I23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>220</v>
       </c>
@@ -915,7 +1050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>221</v>
       </c>
@@ -929,7 +1064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>222</v>
       </c>
@@ -943,7 +1078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>223</v>
       </c>
@@ -957,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>224</v>
       </c>
@@ -971,7 +1106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>225</v>
       </c>
@@ -985,7 +1120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>226</v>
       </c>
@@ -999,7 +1134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>227</v>
       </c>
@@ -1013,7 +1148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>228</v>
       </c>
@@ -1027,7 +1162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>229</v>
       </c>
@@ -1041,7 +1176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>230</v>
       </c>
@@ -1055,7 +1190,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>231</v>
       </c>
@@ -1069,7 +1204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>232</v>
       </c>
@@ -1083,7 +1218,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>233</v>
       </c>
@@ -1097,7 +1232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>234</v>
       </c>
@@ -1111,7 +1246,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>235</v>
       </c>
@@ -1125,7 +1260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>236</v>
       </c>
@@ -1139,7 +1274,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>237</v>
       </c>
@@ -1153,7 +1288,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>238</v>
       </c>
@@ -1167,7 +1302,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>239</v>
       </c>
@@ -1181,7 +1316,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>240</v>
       </c>
@@ -1197,5 +1332,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>